<commit_message>
Further updates and a sample spreadsheet
</commit_message>
<xml_diff>
--- a/example-input/v4_E-MTAB-5061-xtrasmall.xlsx
+++ b/example-input/v4_E-MTAB-5061-xtrasmall.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dwelter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dwelter/Development/HCA/ingest-broker/example-input/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,6 @@
     <sheet name="protocols" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="172">
   <si>
     <t>project_id</t>
   </si>
@@ -310,9 +309,6 @@
     <t>E-MTAB-5061.processed.1.zip</t>
   </si>
   <si>
-    <t>SAMEA4437021</t>
-  </si>
-  <si>
     <t>ERS1348470</t>
   </si>
   <si>
@@ -320,9 +316,6 @@
   </si>
   <si>
     <t>AZ_A7</t>
-  </si>
-  <si>
-    <t>SAMEA4437030</t>
   </si>
   <si>
     <t>ERS1348479</t>
@@ -1381,19 +1374,19 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>64</v>
@@ -1436,10 +1429,10 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
@@ -1469,7 +1462,7 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -1514,19 +1507,19 @@
   <sheetData>
     <row r="1" spans="1:27" ht="29" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="D1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
@@ -1567,28 +1560,28 @@
   <sheetData>
     <row r="1" spans="1:27" ht="43" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="D1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -1612,23 +1605,23 @@
     </row>
     <row r="2" spans="1:27" ht="29" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F2" s="1">
         <v>40000</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -1667,28 +1660,28 @@
   <sheetData>
     <row r="1" spans="1:22" ht="43" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="D1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
@@ -1707,16 +1700,16 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>77</v>
@@ -1753,19 +1746,19 @@
   <sheetData>
     <row r="1" spans="1:27" ht="29" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="D1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
@@ -1808,28 +1801,28 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>64</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="H1" s="14" t="s">
         <v>150</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>152</v>
       </c>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
@@ -1855,26 +1848,26 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>84</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I2" s="2"/>
       <c r="L2" s="2"/>
@@ -1898,26 +1891,26 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>156</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>158</v>
       </c>
       <c r="I3" s="2"/>
       <c r="L3" s="2"/>
@@ -4799,7 +4792,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>2</v>
@@ -4808,50 +4801,50 @@
         <v>4</v>
       </c>
       <c r="D1" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>163</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>166</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>168</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="15" t="s">
         <v>170</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>172</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -6094,7 +6087,7 @@
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6180,14 +6173,12 @@
       <c r="J2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="6"/>
+      <c r="L2" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -6212,7 +6203,7 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>85</v>
@@ -6230,14 +6221,12 @@
       <c r="J3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="K3" s="6" t="s">
-        <v>91</v>
-      </c>
+      <c r="K3" s="6"/>
       <c r="L3" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
@@ -9016,25 +9005,25 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="F1" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="G1" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>64</v>
@@ -9074,16 +9063,16 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>101</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>103</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>64</v>
@@ -9110,7 +9099,7 @@
         <v>69</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
@@ -9143,16 +9132,16 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
Updated time handling and death handling
</commit_message>
<xml_diff>
--- a/example-input/v4_E-MTAB-5061-xtrasmall.xlsx
+++ b/example-input/v4_E-MTAB-5061-xtrasmall.xlsx
@@ -3124,17 +3124,17 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1255060728745"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.753036437247"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8744939271255"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9311740890688"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3168,7 +3168,7 @@
         <v>92</v>
       </c>
       <c r="F2" s="13" t="n">
-        <v>43069.4305555556</v>
+        <v>43044.4305555556</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>83</v>

</xml_diff>